<commit_message>
Update data to 02-06, predict 02-7
</commit_message>
<xml_diff>
--- a/chinancoron2020.xlsx
+++ b/chinancoron2020.xlsx
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -750,6 +750,40 @@
       </c>
       <c r="E21">
         <v>491</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>43866</v>
+      </c>
+      <c r="B22">
+        <v>28060</v>
+      </c>
+      <c r="C22">
+        <v>3697</v>
+      </c>
+      <c r="D22">
+        <v>24702</v>
+      </c>
+      <c r="E22">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>43866</v>
+      </c>
+      <c r="B23">
+        <v>31211</v>
+      </c>
+      <c r="C23">
+        <v>3151</v>
+      </c>
+      <c r="D23">
+        <v>26359</v>
+      </c>
+      <c r="E23">
+        <v>637</v>
       </c>
     </row>
   </sheetData>

</xml_diff>